<commit_message>
try to add a new record in residences.xlsx
residences.xlsx
</commit_message>
<xml_diff>
--- a/residences.xlsx
+++ b/residences.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\residences\directory-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953BECD7-506D-4C84-BA93-F76F2F7F95DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E64993-A9BF-4CB2-9E98-6A9B3426665D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7081FDD0-81F1-4A15-AD6F-A0D08666638A}"/>
+    <workbookView xWindow="696" yWindow="768" windowWidth="30024" windowHeight="12120" xr2:uid="{7081FDD0-81F1-4A15-AD6F-A0D08666638A}"/>
   </bookViews>
   <sheets>
     <sheet name="residences" sheetId="2" r:id="rId1"/>
     <sheet name="del" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">residences!$A$1:$L$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3093" uniqueCount="2093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3094" uniqueCount="2094">
   <si>
     <t>Description</t>
   </si>
@@ -6316,6 +6319,9 @@
   </si>
   <si>
     <t>Assisted Living, BBQ, Billard, Bocce Ball Court, Car Wash, Cinema, Dog Washing Station, Firepit, Fitness Room, Gym, Hobby Room, Kids Area, Locker Rooms, Monthly Activities, Nursing Care, One Bedroom + Den Suites, Onsite Wi-Fi, Parking, Pets' Area, Phone, Physiotherapy, Putting Green, Respite Care, Saltwater Pool, Shuttle Service, Storage, Studio + Den Suites, Studio Suites, Sunroom, TV Room, Two Bedroom Suites</t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
 </sst>
 </file>
@@ -6714,10 +6720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2B0DAE-254D-4FC6-845A-72EEDC5CB68F}">
-  <dimension ref="A1:L336"/>
+  <dimension ref="A1:L337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
-      <selection activeCell="H336" sqref="H336"/>
+    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+      <selection activeCell="B338" sqref="B338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16479,7 +16485,13 @@
         <v>39</v>
       </c>
     </row>
+    <row r="337" spans="1:1">
+      <c r="A337" t="s">
+        <v>2093</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:L1" xr:uid="{9A2B0DAE-254D-4FC6-845A-72EEDC5CB68F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>